<commit_message>
cập nhật tên ảnh và CSDL quan hệ
</commit_message>
<xml_diff>
--- a/VN_FOOD.xlsx
+++ b/VN_FOOD.xlsx
@@ -270,9 +270,6 @@
     <t>Bánh đa cua Hải Phòng</t>
   </si>
   <si>
-    <t>Nem cua bể Haỉ Phòng</t>
-  </si>
-  <si>
     <t>Chả mực Hạ Long</t>
   </si>
   <si>
@@ -482,6 +479,9 @@
   <si>
     <t>phần</t>
   </si>
+  <si>
+    <t>Nem cua bể Hải Phòng</t>
+  </si>
 </sst>
 </file>
 
@@ -489,7 +489,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₫&quot;_-;\-* #,##0.00\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0\ &quot;₫&quot;_-;\-* #,##0\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0\ &quot;₫&quot;_-;\-* #,##0\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -575,19 +575,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -813,8 +813,8 @@
   <dimension ref="A1:Z1005"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A58" sqref="A35:A58"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2123,7 +2123,7 @@
         <v>79</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C35" s="10">
         <v>45000</v>
@@ -2132,7 +2132,7 @@
         <v>7</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
@@ -2161,7 +2161,7 @@
         <v>80</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C36" s="10">
         <v>130000</v>
@@ -2170,7 +2170,7 @@
         <v>7</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
@@ -2199,16 +2199,16 @@
         <v>81</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C37" s="10">
         <v>800000</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
@@ -2237,7 +2237,7 @@
         <v>82</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C38" s="10">
         <v>40000</v>
@@ -2246,7 +2246,7 @@
         <v>7</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
@@ -2272,19 +2272,19 @@
     </row>
     <row r="39" spans="1:26" ht="67.2" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>83</v>
+        <v>153</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C39" s="10">
         <v>200000</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
@@ -2310,19 +2310,19 @@
     </row>
     <row r="40" spans="1:26" ht="84" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C40" s="10">
         <v>450000</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
@@ -2348,19 +2348,19 @@
     </row>
     <row r="41" spans="1:26" ht="100.8" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C41" s="10">
         <v>990000</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
@@ -2386,19 +2386,19 @@
     </row>
     <row r="42" spans="1:26" ht="84" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C42" s="10">
         <v>180000</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
@@ -2424,10 +2424,10 @@
     </row>
     <row r="43" spans="1:26" ht="67.2" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C43" s="10">
         <v>40000</v>
@@ -2436,7 +2436,7 @@
         <v>7</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
@@ -2462,10 +2462,10 @@
     </row>
     <row r="44" spans="1:26" ht="134.4" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C44" s="10">
         <v>30000</v>
@@ -2474,7 +2474,7 @@
         <v>7</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
@@ -2500,10 +2500,10 @@
     </row>
     <row r="45" spans="1:26" ht="84" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C45" s="10">
         <v>45000</v>
@@ -2512,7 +2512,7 @@
         <v>7</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
@@ -2538,10 +2538,10 @@
     </row>
     <row r="46" spans="1:26" ht="100.8" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C46" s="10">
         <v>45000</v>
@@ -2550,7 +2550,7 @@
         <v>7</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
@@ -2576,10 +2576,10 @@
     </row>
     <row r="47" spans="1:26" ht="67.2" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C47" s="10">
         <v>35000</v>
@@ -2588,7 +2588,7 @@
         <v>7</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
@@ -2614,10 +2614,10 @@
     </row>
     <row r="48" spans="1:26" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C48" s="10">
         <v>130000</v>
@@ -2626,7 +2626,7 @@
         <v>7</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
@@ -2652,10 +2652,10 @@
     </row>
     <row r="49" spans="1:26" ht="84" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C49" s="10">
         <v>35000</v>
@@ -2664,7 +2664,7 @@
         <v>7</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
@@ -2690,10 +2690,10 @@
     </row>
     <row r="50" spans="1:26" ht="50.4" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C50" s="10">
         <v>50000</v>
@@ -2702,7 +2702,7 @@
         <v>7</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F50" s="5"/>
       <c r="G50" s="5"/>
@@ -2728,10 +2728,10 @@
     </row>
     <row r="51" spans="1:26" ht="117.6" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C51" s="10">
         <v>20000</v>
@@ -2740,7 +2740,7 @@
         <v>7</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F51" s="5"/>
       <c r="G51" s="5"/>
@@ -2766,10 +2766,10 @@
     </row>
     <row r="52" spans="1:26" ht="67.2" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C52" s="10">
         <v>40000</v>
@@ -2778,7 +2778,7 @@
         <v>7</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F52" s="5"/>
       <c r="G52" s="5"/>
@@ -2804,10 +2804,10 @@
     </row>
     <row r="53" spans="1:26" ht="100.8" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C53" s="10">
         <v>40000</v>
@@ -2816,7 +2816,7 @@
         <v>7</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F53" s="5"/>
       <c r="G53" s="5"/>
@@ -2842,19 +2842,19 @@
     </row>
     <row r="54" spans="1:26" ht="67.2" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C54" s="10">
         <v>10000</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F54" s="5"/>
       <c r="G54" s="5"/>
@@ -2880,10 +2880,10 @@
     </row>
     <row r="55" spans="1:26" ht="67.2" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C55" s="10">
         <v>50000</v>
@@ -2892,7 +2892,7 @@
         <v>7</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F55" s="5"/>
       <c r="G55" s="5"/>
@@ -2918,19 +2918,19 @@
     </row>
     <row r="56" spans="1:26" ht="100.8" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C56" s="10">
         <v>250000</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F56" s="5"/>
       <c r="G56" s="5"/>
@@ -2956,10 +2956,10 @@
     </row>
     <row r="57" spans="1:26" ht="117.6" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C57" s="10">
         <v>20000</v>
@@ -2968,7 +2968,7 @@
         <v>7</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F57" s="5"/>
       <c r="G57" s="5"/>
@@ -2994,10 +2994,10 @@
     </row>
     <row r="58" spans="1:26" ht="67.2" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B58" s="6" t="s">
         <v>101</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>102</v>
       </c>
       <c r="C58" s="10">
         <v>70000</v>
@@ -3006,7 +3006,7 @@
         <v>7</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
@@ -3032,19 +3032,19 @@
     </row>
     <row r="59" spans="1:26" ht="100.8" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C59" s="10">
         <v>15000</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F59" s="5"/>
       <c r="G59" s="5"/>
@@ -3070,19 +3070,19 @@
     </row>
     <row r="60" spans="1:26" ht="117.6" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C60" s="10">
         <v>15000</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F60" s="5"/>
       <c r="G60" s="5"/>
@@ -3108,19 +3108,19 @@
     </row>
     <row r="61" spans="1:26" ht="84" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C61" s="10">
         <v>15000</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
@@ -3146,19 +3146,19 @@
     </row>
     <row r="62" spans="1:26" ht="67.2" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C62" s="10">
         <v>15000</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F62" s="5"/>
       <c r="G62" s="5"/>
@@ -3184,19 +3184,19 @@
     </row>
     <row r="63" spans="1:26" ht="84" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C63" s="10">
         <v>15000</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F63" s="5"/>
       <c r="G63" s="5"/>
@@ -3222,19 +3222,19 @@
     </row>
     <row r="64" spans="1:26" ht="50.4" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C64" s="10">
         <v>35000</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F64" s="5"/>
       <c r="G64" s="5"/>
@@ -3260,19 +3260,19 @@
     </row>
     <row r="65" spans="1:26" ht="67.2" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C65" s="10">
         <v>20000</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F65" s="5"/>
       <c r="G65" s="5"/>
@@ -3298,19 +3298,19 @@
     </row>
     <row r="66" spans="1:26" ht="84" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C66" s="10">
         <v>25000</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F66" s="5"/>
       <c r="G66" s="5"/>
@@ -3336,19 +3336,19 @@
     </row>
     <row r="67" spans="1:26" ht="67.2" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C67" s="10">
         <v>15000</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F67" s="5"/>
       <c r="G67" s="5"/>
@@ -3374,19 +3374,19 @@
     </row>
     <row r="68" spans="1:26" ht="50.4" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C68" s="10">
         <v>15000</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F68" s="5"/>
       <c r="G68" s="5"/>

</xml_diff>